<commit_message>
primera versión del censuses
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\cursos\asw\LoadUsers\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohanArif\Documents\Universidad\Cuarto Curso\ASW\censuses\censuses_3b\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Colegio</t>
   </si>
   <si>
-    <t>Mesa</t>
-  </si>
-  <si>
     <t>NIF</t>
   </si>
   <si>
@@ -54,16 +51,36 @@
   </si>
   <si>
     <t>09940449X</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>a@gmail.com</t>
+  </si>
+  <si>
+    <t>b@gmail.com</t>
+  </si>
+  <si>
+    <t>c@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,14 +103,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -375,7 +395,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,64 +403,69 @@
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>234</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>345</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>345</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <v>456</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Parsear la hoja de calculo y division en algunos paquetes
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nombre</t>
   </si>
@@ -51,36 +51,16 @@
   </si>
   <si>
     <t>09940449X</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>a@gmail.com</t>
-  </si>
-  <si>
-    <t>b@gmail.com</t>
-  </si>
-  <si>
-    <t>c@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,17 +83,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +380,7 @@
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,61 +388,44 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>456</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios en RCensus y excel
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cecilia\Desktop\CENSUSES\censuses_3b-master\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8376" windowHeight="2376"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8370" windowHeight="2370"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -51,19 +46,38 @@
   </si>
   <si>
     <t>09940449X</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>juan@gmail.com</t>
+  </si>
+  <si>
+    <t>luis@gmail.com</t>
+  </si>
+  <si>
+    <t>ana@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,14 +97,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -149,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,7 +204,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,26 +381,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,44 +408,61 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <v>456</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>